<commit_message>
Fix typo in master file (fixed already in read-in file)
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
+++ b/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="4620" windowWidth="25040" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="13200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -236,8 +236,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,7 +326,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -357,6 +361,8 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -391,6 +397,8 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1104,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F27">
         <f>0.15%</f>
@@ -1181,7 +1189,7 @@
         <v>12</v>
       </c>
       <c r="E28">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F28">
         <f>0.15%</f>
@@ -1266,59 +1274,59 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G29">
-        <f>LOOKUP(RIGHT(G26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G29:T29" si="1">LOOKUP(RIGHT(G26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H29">
-        <f>LOOKUP(RIGHT(H26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I29">
-        <f>LOOKUP(RIGHT(I26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J29">
-        <f>LOOKUP(RIGHT(J26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K29">
-        <f>LOOKUP(RIGHT(K26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L29">
-        <f>LOOKUP(RIGHT(L26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M29">
-        <f>LOOKUP(RIGHT(M26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N29">
-        <f>LOOKUP(RIGHT(N26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O29">
-        <f>LOOKUP(RIGHT(O26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P29">
-        <f>LOOKUP(RIGHT(P26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q29">
-        <f>LOOKUP(RIGHT(Q26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R29">
-        <f>LOOKUP(RIGHT(R26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S29">
-        <f>LOOKUP(RIGHT(S26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T29">
-        <f>LOOKUP(RIGHT(T26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="1"/>
         <v>2.46E-2</v>
       </c>
     </row>
@@ -1344,59 +1352,59 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:T30" si="1">LOOKUP(RIGHT(G$26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G30:T30" si="2">LOOKUP(RIGHT(G$26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.46E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update shipping fuel sulfur contents.
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
+++ b/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D3K117/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/default-emissions-data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A030B9C8-5598-4541-8DBD-94273D7927EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="4040" windowWidth="23920" windowHeight="13200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2420" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,19 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,8 +38,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D58DFB88-230A-1643-A2E9-F1165F20800C}</author>
+  </authors>
+  <commentList>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{D58DFB88-230A-1643-A2E9-F1165F20800C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    3-year average</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Resid S%</t>
   </si>
@@ -144,9 +179,6 @@
     <t>SO2</t>
   </si>
   <si>
-    <t>IMO Sulphur monitoring. Heavy oil S% adjusted before 2009 for mass/sample weighted bias. Distillate S% assumed to linearly approahc 5000 ppm by 1990</t>
-  </si>
-  <si>
     <t>X1990</t>
   </si>
   <si>
@@ -163,13 +195,55 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Ref: IMO - Sulphur monitoring for 2017 (IMO)</t>
+  </si>
+  <si>
+    <t>Ref: MEPC-74-18-Report-Of-The-Marine-Environment-Protection-Committee On-Its-Seventy-Fourth-Session-Secretariat</t>
+  </si>
+  <si>
+    <t>New Limit:</t>
+  </si>
+  <si>
+    <t>% in compliance ( Diamond et al. 2023 in press, pers com)</t>
+  </si>
+  <si>
+    <t>* Assume complimant fraction is at limit. Assume non-compliant fraction is at recent global average.</t>
+  </si>
+  <si>
+    <t>X2015</t>
+  </si>
+  <si>
+    <t>X2016</t>
+  </si>
+  <si>
+    <t>X2017</t>
+  </si>
+  <si>
+    <t>X2018</t>
+  </si>
+  <si>
+    <t>X2019</t>
+  </si>
+  <si>
+    <t>X2020</t>
+  </si>
+  <si>
+    <t>X2021</t>
+  </si>
+  <si>
+    <t>X2022</t>
+  </si>
+  <si>
+    <t>IMO Sulphur monitoring. Heavy oil S% adjusted before 2009 for mass/sample weighted bias. Distillate S% assumed to linearly approahc 5000 ppm by 1990, ramping down to IMO estimated levels after 2911. 2020 forward estimates based on fraction of fuel oil reported to be in compliance (as reported by Diamond et al. 2023, in press).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,11 +277,31 @@
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Times"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -311,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,6 +419,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -403,18 +505,26 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Data"/>
       <sheetName val="Emissions Proxy"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="3">
           <cell r="B3">
             <v>2.7E-2</v>
@@ -494,10 +604,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Smith, Steven J (PNNL-JGCRI)" id="{4A648797-47A4-FC4A-B01E-21D5644D1305}" userId="S::ssmith@pnnl.gov::bb1e00e9-e65d-4911-8fc9-cd876d8ab9b6" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -820,22 +936,30 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B21" dT="2020-04-27T03:27:15.71" personId="{4A648797-47A4-FC4A-B01E-21D5644D1305}" id="{D58DFB88-230A-1643-A2E9-F1165F20800C}">
+    <text>3-year average</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A41" sqref="A38:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="20" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -846,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -858,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -870,7 +994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -882,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -894,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -906,7 +1030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -918,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -930,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -942,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -954,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -966,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -978,7 +1102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -990,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -1002,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -1014,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -1026,452 +1150,720 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="4" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.46E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2015</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2016</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2.58E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2017</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2019</v>
+      </c>
+      <c r="B22" s="9">
+        <f>B21</f>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2020</v>
+      </c>
+      <c r="B23" s="2">
+        <f>D23+E23</f>
+        <v>8.7799999999999996E-3</v>
+      </c>
+      <c r="D23" s="10">
+        <f>$K$23*G23</f>
+        <v>4.0999999999999995E-3</v>
+      </c>
+      <c r="E23" s="10">
+        <f>(1-G23)*$B$20</f>
+        <v>4.680000000000001E-3</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2021</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" ref="B24:B25" si="0">D24+E24</f>
+        <v>9.8299999999999985E-3</v>
+      </c>
+      <c r="D24" s="10">
+        <f>$K$23*G24</f>
+        <v>3.8500000000000001E-3</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" ref="E24:E25" si="1">(1-G24)*$B$20</f>
+        <v>5.9799999999999992E-3</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2022</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0460000000000001E-2</v>
+      </c>
+      <c r="D25" s="10">
+        <f>$K$23*G25</f>
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="1"/>
+        <v>6.7599999999999995E-3</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F28" s="10"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="5" t="s">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB37" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F38">
+        <f>0.15%</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:V39" si="2">0.15%</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="Q38">
+        <v>1.5E-3</v>
+      </c>
+      <c r="R38">
+        <v>1.4E-3</v>
+      </c>
+      <c r="S38">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="T38">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="U38">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="V38">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="W38">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="X38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="Y38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="Z38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AA38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F39">
+        <f>0.15%</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="Q39">
+        <v>1.5E-3</v>
+      </c>
+      <c r="R39">
+        <v>1.4E-3</v>
+      </c>
+      <c r="S39">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="T39">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="U39">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="V39">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="W39">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="X39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="Y39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="Z39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AA39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <f>F40</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="F40">
+        <f>LOOKUP(RIGHT(F$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:T40" si="3">LOOKUP(RIGHT(G37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>2.8765957446808512E-2</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="3"/>
+        <v>2.8655319148936171E-2</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>2.6774468085106383E-2</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="3"/>
+        <v>2.6221276595744681E-2</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="3"/>
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="3"/>
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="T40">
+        <f>LOOKUP(RIGHT(T37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
+        <v>2.46E-2</v>
+      </c>
+      <c r="U40">
+        <f t="shared" ref="U40:AB40" si="4">LOOKUP(RIGHT(U37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="4"/>
+        <v>2.58E-2</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="4"/>
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="4"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="4"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="4"/>
+        <v>8.7799999999999996E-3</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="4"/>
+        <v>9.8299999999999985E-3</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="4"/>
+        <v>1.0460000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <f>F41</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="F41">
+        <f>LOOKUP(RIGHT(F$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="G41">
+        <f>LOOKUP(RIGHT(G$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="H41">
+        <f>LOOKUP(RIGHT(H$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.8765957446808512E-2</v>
+      </c>
+      <c r="I41">
+        <f>LOOKUP(RIGHT(I$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="J41">
+        <f>LOOKUP(RIGHT(J$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="K41">
+        <f>LOOKUP(RIGHT(K$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.9872340425531916E-2</v>
+      </c>
+      <c r="L41">
+        <f>LOOKUP(RIGHT(L$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.8655319148936171E-2</v>
+      </c>
+      <c r="M41">
+        <f>LOOKUP(RIGHT(M$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.6774468085106383E-2</v>
+      </c>
+      <c r="N41">
+        <f>LOOKUP(RIGHT(N$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.6221276595744681E-2</v>
+      </c>
+      <c r="O41">
+        <f>LOOKUP(RIGHT(O$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="P41">
+        <f>LOOKUP(RIGHT(P$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="Q41">
+        <f>LOOKUP(RIGHT(Q$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="R41">
+        <f>LOOKUP(RIGHT(R$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="S41">
+        <f>LOOKUP(RIGHT(S$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="T41">
+        <f>T40</f>
+        <v>2.46E-2</v>
+      </c>
+      <c r="U41">
+        <f t="shared" ref="U41:AB41" si="5">U40</f>
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="5"/>
+        <v>2.58E-2</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="5"/>
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="5"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="5"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="5"/>
+        <v>8.7799999999999996E-3</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="5"/>
+        <v>9.8299999999999985E-3</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="5"/>
+        <v>1.0460000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" t="s">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
         <v>10</v>
       </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F27">
-        <f>0.15%</f>
-        <v>1.5E-3</v>
-      </c>
-      <c r="G27">
-        <f t="shared" ref="G27:T28" si="0">0.15%</f>
-        <v>1.5E-3</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F28">
-        <f>0.15%</f>
-        <v>1.5E-3</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="0"/>
-        <v>1.5E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29">
-        <f>F29</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="F29">
-        <f>LOOKUP(RIGHT(F$26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="G29">
-        <f t="shared" ref="G29:T29" si="1">LOOKUP(RIGHT(G26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
-        <v>2.8765957446808512E-2</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="1"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="1"/>
-        <v>2.8655319148936171E-2</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="1"/>
-        <v>2.6774468085106383E-2</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="1"/>
-        <v>2.6221276595744681E-2</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="1"/>
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>2.6499999999999999E-2</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="1"/>
-        <v>2.5100000000000001E-2</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="1"/>
-        <v>2.4299999999999999E-2</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="1"/>
-        <v>2.46E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30">
-        <f>F30</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="F30">
-        <f>LOOKUP(RIGHT(F$26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="G30">
-        <f t="shared" ref="G30:T30" si="2">LOOKUP(RIGHT(G$26,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="2"/>
-        <v>2.8765957446808512E-2</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="2"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="2"/>
-        <v>2.9872340425531916E-2</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="2"/>
-        <v>2.8655319148936171E-2</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="2"/>
-        <v>2.6774468085106383E-2</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="2"/>
-        <v>2.6221276595744681E-2</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="2"/>
-        <v>2.6000000000000002E-2</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="2"/>
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="2"/>
-        <v>2.6499999999999999E-2</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="2"/>
-        <v>2.5100000000000001E-2</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="2"/>
-        <v>2.4299999999999999E-2</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="2"/>
-        <v>2.46E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="B33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="D48" t="s">
         <v>37</v>
       </c>
-      <c r="E37">
+      <c r="E48">
         <v>2000</v>
       </c>
-      <c r="F37">
+      <c r="F48">
         <v>2014</v>
       </c>
-      <c r="G37" t="s">
-        <v>40</v>
+      <c r="G48" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Shipping and metals update to 2022 (#420)
* Update shipping fuel use, and metal SO2 emissions
* Commit lower Al SO2 emission factor for Qatar smelter due to seawater scrubbing.
* Add new Al production data
* Made aluminum production activity code more robust by removing hard coded year and adding logic to truncate or extend forward
* Update Al production data and associated mapping file
* Update default estimate. Removes Al smelting, revises Serbia and Zambia time series.
* Typo correction
* Changed capitalization to what's used in S1.1
* Remove superfluous TODO comment (is done).

---------

Co-authored-by: Steve Smith <ssmith@pnnl.gov>
Co-authored-by: hahsan1 <72406931+hahsan1@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
+++ b/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D3K117/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/default-emissions-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3k117/Downloads/git-repos/CEDS-master/input/default-emissions-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A030B9C8-5598-4541-8DBD-94273D7927EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFAD2B-D594-9A4B-8801-A9AABFD1D87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2420" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="760" windowWidth="28120" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Resid S%</t>
   </si>
@@ -206,9 +206,6 @@
     <t>New Limit:</t>
   </si>
   <si>
-    <t>% in compliance ( Diamond et al. 2023 in press, pers com)</t>
-  </si>
-  <si>
     <t>* Assume complimant fraction is at limit. Assume non-compliant fraction is at recent global average.</t>
   </si>
   <si>
@@ -236,14 +233,33 @@
     <t>X2022</t>
   </si>
   <si>
-    <t>IMO Sulphur monitoring. Heavy oil S% adjusted before 2009 for mass/sample weighted bias. Distillate S% assumed to linearly approahc 5000 ppm by 1990, ramping down to IMO estimated levels after 2911. 2020 forward estimates based on fraction of fuel oil reported to be in compliance (as reported by Diamond et al. 2023, in press).</t>
+    <t>Fract with scrubbers</t>
+  </si>
+  <si>
+    <t>Global scrubber washwater discharges under IMO’s 2020 fuel sulfur limit (Osipova etal 2021)</t>
+  </si>
+  <si>
+    <t>S% in compliance ( Diamond et al. 2023. doi: 10.5194/acp-23-8259-2023)</t>
+  </si>
+  <si>
+    <t>BNF (https://www.bloomberg.com/news/articles/2019-01-17/how-the-cargo-ship-industry-is-cleaning-up-its-filthy-act, 12/26/2023)</t>
+  </si>
+  <si>
+    <t>Total compliance (Low S% + scrubbers)</t>
+  </si>
+  <si>
+    <t>Third IMO GHG Study 2014 (MEPC-67-6-INF3-2014); IMO - Sulphur monitoring - various years; Fourth IMO GHG Study 2020 (MEPC 75-7-15); IMO Sulphur monitoring. Heavy oil S% adjusted before 2009 for mass/sample weighted bias. Distillate S% assumed to linearly approach 5000 ppm by 1990; ramping down to IMO estimated levels after 2911. 2020 forward estimates based on fraction of fuel oil reported to be in compliance (as reported by Diamond et al. 2023 doi: 10.5194/acp-23-8259-2023) + estimate of number of ships with scrubbers (Osipova etal 2021)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,12 +302,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -302,6 +312,24 @@
       <sz val="8"/>
       <name val="Times"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +358,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,8 +432,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,12 +452,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="73" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="73" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -502,6 +535,7 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="73" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -948,18 +982,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A41" sqref="A38:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="P14" workbookViewId="0">
+      <selection activeCell="Z40" sqref="Z40:AB41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="20" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -970,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -982,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -994,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -1006,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -1018,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -1030,7 +1064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1042,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -1054,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -1066,7 +1100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -1078,7 +1112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -1090,7 +1124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -1102,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -1114,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -1126,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -1138,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -1150,7 +1184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -1158,7 +1192,7 @@
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -1169,7 +1203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -1180,7 +1214,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -1191,7 +1225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -1201,8 +1235,11 @@
       <c r="C21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S21" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1211,27 +1248,31 @@
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="P22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>2020</v>
       </c>
       <c r="B23" s="2">
         <f>D23+E23</f>
-        <v>8.7799999999999996E-3</v>
+        <v>7.8428436473670631E-3</v>
       </c>
       <c r="D23" s="10">
         <f>$K$23*G23</f>
-        <v>4.0999999999999995E-3</v>
+        <v>4.3231324649126044E-3</v>
       </c>
       <c r="E23" s="10">
         <f>(1-G23)*$B$20</f>
-        <v>4.680000000000001E-3</v>
+        <v>3.5197111824544587E-3</v>
       </c>
       <c r="G23" s="8">
-        <v>0.82</v>
+        <f>P23+S23</f>
+        <v>0.86462649298252081</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>48</v>
@@ -1239,66 +1280,118 @@
       <c r="K23" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P23" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="S23" s="12">
+        <f>3628/81297</f>
+        <v>4.4626492982520881E-2</v>
+      </c>
+      <c r="T23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>2021</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B25" si="0">D24+E24</f>
-        <v>9.8299999999999985E-3</v>
+        <v>8.8322952876489919E-3</v>
       </c>
       <c r="D24" s="10">
         <f>$K$23*G24</f>
-        <v>3.8500000000000001E-3</v>
+        <v>4.0875487410359547E-3</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" ref="E24:E25" si="1">(1-G24)*$B$20</f>
-        <v>5.9799999999999992E-3</v>
+        <v>4.7447465466130363E-3</v>
       </c>
       <c r="G24" s="8">
+        <f t="shared" ref="G24:G25" si="2">P24+S24</f>
+        <v>0.81750974820719091</v>
+      </c>
+      <c r="P24" s="8">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S24" s="13">
+        <f>S23+($S$28-$S$23)/5</f>
+        <v>4.7509748207190915E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>2022</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
-        <v>1.0460000000000001E-2</v>
+        <v>9.4017469279309204E-3</v>
       </c>
       <c r="D25" s="10">
         <f>$K$23*G25</f>
-        <v>3.7000000000000002E-3</v>
+        <v>3.9519650171593044E-3</v>
       </c>
       <c r="E25" s="10">
         <f t="shared" si="1"/>
-        <v>6.7599999999999995E-3</v>
+        <v>5.449781910771616E-3</v>
       </c>
       <c r="G25" s="8">
+        <f t="shared" si="2"/>
+        <v>0.79039300343186092</v>
+      </c>
+      <c r="P25" s="8">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S25" s="13">
+        <f t="shared" ref="S25:S27" si="3">S24+($S$28-$S$23)/5</f>
+        <v>5.0393003431860948E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26">
+        <v>2023</v>
+      </c>
       <c r="D26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="S26" s="13">
+        <f t="shared" si="3"/>
+        <v>5.3276258656530982E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="S27" s="13">
+        <f t="shared" si="3"/>
+        <v>5.6159513881201016E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28">
+        <v>2025</v>
+      </c>
       <c r="F28" s="10"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S28" s="12">
+        <f>4800/81297</f>
+        <v>5.9042769105871064E-2</v>
+      </c>
+      <c r="T28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28">
       <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
@@ -1360,31 +1453,31 @@
         <v>28</v>
       </c>
       <c r="U37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="V37" s="3" t="s">
+      <c r="W37" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W37" s="3" t="s">
+      <c r="X37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="X37" s="3" t="s">
+      <c r="Y37" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Y37" s="3" t="s">
+      <c r="Z37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Z37" s="3" t="s">
+      <c r="AA37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA37" s="3" t="s">
+      <c r="AB37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AB37" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1405,43 +1498,43 @@
         <v>1.5E-3</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:V39" si="2">0.15%</f>
+        <f t="shared" ref="G38:P39" si="4">0.15%</f>
         <v>1.5E-3</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="I38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="J38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="L38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="M38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="N38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="O38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="P38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="Q38">
@@ -1481,7 +1574,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1502,43 +1595,43 @@
         <v>1.5E-3</v>
       </c>
       <c r="G39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="I39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="J39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="L39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="M39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="N39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="O39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="P39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="Q39">
@@ -1578,7 +1671,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1600,55 +1693,55 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40:T40" si="3">LOOKUP(RIGHT(G37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G40:S40" si="5">LOOKUP(RIGHT(G37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T40">
@@ -1656,39 +1749,39 @@
         <v>2.46E-2</v>
       </c>
       <c r="U40">
-        <f t="shared" ref="U40:AB40" si="4">LOOKUP(RIGHT(U37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
+        <f t="shared" ref="U40:AB40" si="6">LOOKUP(RIGHT(U37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="V40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.58E-2</v>
       </c>
       <c r="W40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="X40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="Z40">
-        <f t="shared" si="4"/>
-        <v>8.7799999999999996E-3</v>
-      </c>
-      <c r="AA40">
-        <f t="shared" si="4"/>
-        <v>9.8299999999999985E-3</v>
-      </c>
-      <c r="AB40">
-        <f t="shared" si="4"/>
-        <v>1.0460000000000001E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="Z40" s="14">
+        <f t="shared" si="6"/>
+        <v>7.8428436473670631E-3</v>
+      </c>
+      <c r="AA40" s="14">
+        <f t="shared" si="6"/>
+        <v>8.8322952876489919E-3</v>
+      </c>
+      <c r="AB40" s="14">
+        <f t="shared" si="6"/>
+        <v>9.4017469279309204E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1710,55 +1803,55 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G41">
-        <f>LOOKUP(RIGHT(G$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G41:S41" si="7">LOOKUP(RIGHT(G$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H41">
-        <f>LOOKUP(RIGHT(H$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I41">
-        <f>LOOKUP(RIGHT(I$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J41">
-        <f>LOOKUP(RIGHT(J$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K41">
-        <f>LOOKUP(RIGHT(K$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L41">
-        <f>LOOKUP(RIGHT(L$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M41">
-        <f>LOOKUP(RIGHT(M$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N41">
-        <f>LOOKUP(RIGHT(N$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O41">
-        <f>LOOKUP(RIGHT(O$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P41">
-        <f>LOOKUP(RIGHT(P$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q41">
-        <f>LOOKUP(RIGHT(Q$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R41">
-        <f>LOOKUP(RIGHT(R$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S41">
-        <f>LOOKUP(RIGHT(S$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" si="7"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T41">
@@ -1766,54 +1859,54 @@
         <v>2.46E-2</v>
       </c>
       <c r="U41">
-        <f t="shared" ref="U41:AB41" si="5">U40</f>
+        <f t="shared" ref="U41:AB41" si="8">U40</f>
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="V41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.58E-2</v>
       </c>
       <c r="W41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="X41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="Z41">
-        <f t="shared" si="5"/>
-        <v>8.7799999999999996E-3</v>
-      </c>
-      <c r="AA41">
-        <f t="shared" si="5"/>
-        <v>9.8299999999999985E-3</v>
-      </c>
-      <c r="AB41">
-        <f t="shared" si="5"/>
-        <v>1.0460000000000001E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="Z41" s="14">
+        <f t="shared" si="8"/>
+        <v>7.8428436473670631E-3</v>
+      </c>
+      <c r="AA41" s="14">
+        <f t="shared" si="8"/>
+        <v>8.8322952876489919E-3</v>
+      </c>
+      <c r="AB41" s="14">
+        <f t="shared" si="8"/>
+        <v>9.4017469279309204E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28">
       <c r="B44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28">
       <c r="A46" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -1836,7 +1929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -1856,11 +1949,11 @@
         <v>2014</v>
       </c>
       <c r="G48" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
March 18, 2025 release - Update to latest IEA and Energy Institute energy consumption data - Update default emissions data to EDGAR v8.1 (air pollutants to 2012), EDGAR_2024_GHG (CH4, N2O to 2023), latest FAO (agriculture CH4 and N2O to 2022), Andrew (CO2 cement to 2024) - Updated inventory data for Australia, Canada, EMEP, UNFCCC (Annex I GHGs), Japan and Korea via HTAPv3.1, and United States. - Updated BOCOC scaling via EDGAR for USA, Canada, and larger European and Asian countries for road and building emissions. - Update to latest OMI/TropOMI composite SO2 point source catalog (through 2022). - Update coal sulfur content and sulfur control in Asia. - Adjust historical EF extension to increase low BC/OC EFs to match premodern SPEW values. - Correct errant Russian flaring values. - Numerous country and sector-specific updates.
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
+++ b/input/default-emissions-data/Shipping_Sulfur_Content.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3k117/Downloads/git-repos/CEDS-master/input/default-emissions-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3k117/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/default-emissions-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFAD2B-D594-9A4B-8801-A9AABFD1D87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F326ACD6-4B3D-AB47-ADB4-EC225D2FB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="760" windowWidth="28120" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Scrubber % Adjustment" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="100">
   <si>
     <t>Resid S%</t>
   </si>
@@ -249,6 +250,115 @@
   </si>
   <si>
     <t>Third IMO GHG Study 2014 (MEPC-67-6-INF3-2014); IMO - Sulphur monitoring - various years; Fourth IMO GHG Study 2020 (MEPC 75-7-15); IMO Sulphur monitoring. Heavy oil S% adjusted before 2009 for mass/sample weighted bias. Distillate S% assumed to linearly approach 5000 ppm by 1990; ramping down to IMO estimated levels after 2911. 2020 forward estimates based on fraction of fuel oil reported to be in compliance (as reported by Diamond et al. 2023 doi: 10.5194/acp-23-8259-2023) + estimate of number of ships with scrubbers (Osipova etal 2021)</t>
+  </si>
+  <si>
+    <t>Total CO2</t>
+  </si>
+  <si>
+    <t>Bulk carrier</t>
+  </si>
+  <si>
+    <t>Chemical tanker</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>General cargo</t>
+  </si>
+  <si>
+    <t>Liquefied gas tanker</t>
+  </si>
+  <si>
+    <t>Oil tanker</t>
+  </si>
+  <si>
+    <t>Other liquids tankers</t>
+  </si>
+  <si>
+    <t>Ferry-pax only</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Ferry-RoPax</t>
+  </si>
+  <si>
+    <t>Refrigerated bulk</t>
+  </si>
+  <si>
+    <t>Ro-Ro</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Yacht</t>
+  </si>
+  <si>
+    <t>Service - tug</t>
+  </si>
+  <si>
+    <t>Miscellaneous -
+fishing</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Service - other</t>
+  </si>
+  <si>
+    <t>Miscellaneous - other</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Source: 4th IMO GHG report table 35</t>
+  </si>
+  <si>
+    <t>bulk carriers</t>
+  </si>
+  <si>
+    <t>container vessels</t>
+  </si>
+  <si>
+    <t>crude oil and product tankers</t>
+  </si>
+  <si>
+    <t>cruise ships</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>% Scrubber</t>
+  </si>
+  <si>
+    <t>CO2 Emissions (proxy for fuel consumption) by ship type (2018)</t>
+  </si>
+  <si>
+    <t>* This is raw fraction relative to number of large vessels</t>
+  </si>
+  <si>
+    <t>Index to fraction of fuel for 2022, last year of Hermansson etal 2024 data</t>
+  </si>
+  <si>
+    <t>Aprox fract of fuel consumption by ships with scrubbers</t>
+  </si>
+  <si>
+    <t>X2023</t>
+  </si>
+  <si>
+    <t>Estimated % of fuel used on ship with scrubbers:</t>
+  </si>
+  <si>
+    <t>Distribution of SO2 Scrubbers (Source: Hermansson etal 2024*)</t>
+  </si>
+  <si>
+    <t>* Hermansson etal (2024), Strong economic incentives of ship scrubbers promoting pollution. https://doi.org/10.1038/s41893-024-01347-1</t>
   </si>
 </sst>
 </file>
@@ -257,7 +367,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -434,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,7 +569,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="73" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="73" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="73" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -980,10 +1097,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB48"/>
+  <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P14" workbookViewId="0">
-      <selection activeCell="Z40" sqref="Z40:AB41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AC40" sqref="Z40:AC40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1184,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -1192,7 +1312,7 @@
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -1203,7 +1323,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -1214,7 +1334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -1225,7 +1345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -1236,10 +1356,13 @@
         <v>47</v>
       </c>
       <c r="S21" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y21" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -1254,25 +1377,25 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>2020</v>
       </c>
       <c r="B23" s="2">
         <f>D23+E23</f>
-        <v>7.8428436473670631E-3</v>
+        <v>4.973301266935984E-3</v>
       </c>
       <c r="D23" s="10">
         <f>$K$23*G23</f>
-        <v>4.3231324649126044E-3</v>
+        <v>5.0063568412057179E-3</v>
       </c>
       <c r="E23" s="10">
         <f>(1-G23)*$B$20</f>
-        <v>3.5197111824544587E-3</v>
+        <v>-3.3055574269733601E-5</v>
       </c>
       <c r="G23" s="8">
         <f>P23+S23</f>
-        <v>0.86462649298252081</v>
+        <v>1.0012713682411436</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>48</v>
@@ -1283,115 +1406,210 @@
       <c r="P23" s="8">
         <v>0.82</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="13">
+        <f>$S$25*Y23/$Y$25</f>
+        <v>0.18127136824114365</v>
+      </c>
+      <c r="Y23" s="12">
         <f>3628/81297</f>
         <v>4.4626492982520881E-2</v>
       </c>
-      <c r="T23" t="s">
+      <c r="Z23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>2021</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" ref="B24:B25" si="0">D24+E24</f>
-        <v>8.8322952876489919E-3</v>
+        <f t="shared" ref="B24:B28" si="0">D24+E24</f>
+        <v>5.7773557920103493E-3</v>
       </c>
       <c r="D24" s="10">
         <f>$K$23*G24</f>
-        <v>4.0875487410359547E-3</v>
+        <v>4.8149152876165837E-3</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" ref="E24:E25" si="1">(1-G24)*$B$20</f>
-        <v>4.7447465466130363E-3</v>
+        <v>9.6244050439376575E-4</v>
       </c>
       <c r="G24" s="8">
-        <f t="shared" ref="G24:G25" si="2">P24+S24</f>
-        <v>0.81750974820719091</v>
+        <f t="shared" ref="G24" si="2">P24+S24</f>
+        <v>0.9629830575233167</v>
       </c>
       <c r="P24" s="8">
         <v>0.77</v>
       </c>
       <c r="S24" s="13">
-        <f>S23+($S$28-$S$23)/5</f>
+        <f>$S$25*Y24/$Y$25</f>
+        <v>0.19298305752331674</v>
+      </c>
+      <c r="Y24" s="13">
+        <f>Y23+($Y$28-$Y$23)/5</f>
         <v>4.7509748207190915E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>2022</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
-        <v>9.4017469279309204E-3</v>
+        <v>6.1614103170847135E-3</v>
       </c>
       <c r="D25" s="10">
         <f>$K$23*G25</f>
-        <v>3.9519650171593044E-3</v>
+        <v>4.7234737340274488E-3</v>
       </c>
       <c r="E25" s="10">
         <f t="shared" si="1"/>
-        <v>5.449781910771616E-3</v>
+        <v>1.4379365830572647E-3</v>
       </c>
       <c r="G25" s="8">
-        <f t="shared" si="2"/>
-        <v>0.79039300343186092</v>
+        <f>P25+S25</f>
+        <v>0.94469474680548982</v>
       </c>
       <c r="P25" s="8">
         <v>0.74</v>
       </c>
       <c r="S25" s="13">
-        <f t="shared" ref="S25:S27" si="3">S24+($S$28-$S$23)/5</f>
+        <f>'Scrubber % Adjustment'!$I$9</f>
+        <v>0.20469474680548982</v>
+      </c>
+      <c r="Y25" s="13">
+        <f t="shared" ref="Y25:Y27" si="3">Y24+($Y$28-$Y$23)/5</f>
         <v>5.0393003431860948E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>2023</v>
       </c>
-      <c r="D26" t="s">
-        <v>49</v>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>5.9154648421590773E-3</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" ref="D26:D28" si="4">$K$23*G26</f>
+        <v>4.7820321804383148E-3</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" ref="E26:E28" si="5">(1-G26)*$B$20</f>
+        <v>1.133432661720763E-3</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" ref="G26:G28" si="6">P26+S26</f>
+        <v>0.95640643608766296</v>
+      </c>
+      <c r="P26" s="8">
+        <f>P25</f>
+        <v>0.74</v>
       </c>
       <c r="S26" s="13">
+        <f t="shared" ref="S26:S28" si="7">$S$25*Y26/$Y$25</f>
+        <v>0.21640643608766291</v>
+      </c>
+      <c r="Y26" s="13">
         <f t="shared" si="3"/>
         <v>5.3276258656530982E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>2024</v>
       </c>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>5.669519367233442E-3</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="4"/>
+        <v>4.8405906268491807E-3</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="5"/>
+        <v>8.2892874038426132E-4</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="6"/>
+        <v>0.9681181253698361</v>
+      </c>
+      <c r="P27" s="8">
+        <f t="shared" ref="P27:P28" si="8">P26</f>
+        <v>0.74</v>
+      </c>
       <c r="S27" s="13">
+        <f t="shared" si="7"/>
+        <v>0.22811812536983606</v>
+      </c>
+      <c r="Y27" s="13">
         <f t="shared" si="3"/>
         <v>5.6159513881201016E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>2025</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="S28" s="12">
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>5.4235738923078067E-3</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="4"/>
+        <v>4.8991490732600467E-3</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="5"/>
+        <v>5.2442481904775963E-4</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="6"/>
+        <v>0.97982981465200925</v>
+      </c>
+      <c r="P28" s="8">
+        <f t="shared" si="8"/>
+        <v>0.74</v>
+      </c>
+      <c r="S28" s="13">
+        <f t="shared" si="7"/>
+        <v>0.2398298146520092</v>
+      </c>
+      <c r="Y28" s="12">
         <f>4800/81297</f>
         <v>5.9042769105871064E-2</v>
       </c>
-      <c r="T28" t="s">
+      <c r="Z28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="29" spans="1:26">
+      <c r="Y29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="S30" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:29">
       <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:29">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
@@ -1476,8 +1694,11 @@
       <c r="AB37" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:28">
+      <c r="AC37" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1498,43 +1719,43 @@
         <v>1.5E-3</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:P39" si="4">0.15%</f>
+        <f t="shared" ref="G38:P39" si="9">0.15%</f>
         <v>1.5E-3</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="I38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="J38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="K38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="L38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="M38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="N38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="O38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="P38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="Q38">
@@ -1573,8 +1794,11 @@
       <c r="AB38">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:28">
+      <c r="AC38">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1595,43 +1819,43 @@
         <v>1.5E-3</v>
       </c>
       <c r="G39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="I39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="J39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="K39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="L39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="M39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="N39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="O39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="P39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5E-3</v>
       </c>
       <c r="Q39">
@@ -1670,8 +1894,11 @@
       <c r="AB39">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="40" spans="1:28">
+      <c r="AC39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1693,55 +1920,55 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40:S40" si="5">LOOKUP(RIGHT(G37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G40:S40" si="10">LOOKUP(RIGHT(G37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T40">
@@ -1749,39 +1976,43 @@
         <v>2.46E-2</v>
       </c>
       <c r="U40">
-        <f t="shared" ref="U40:AB40" si="6">LOOKUP(RIGHT(U37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
+        <f t="shared" ref="U40:Y40" si="11">LOOKUP(RIGHT(U37,4)*1, $A$2:$A$25,$B$2:$B$25)</f>
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="V40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.58E-2</v>
       </c>
       <c r="W40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="X40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Z40" s="14">
-        <f t="shared" si="6"/>
-        <v>7.8428436473670631E-3</v>
+        <f t="shared" ref="Z40:AB40" si="12">LOOKUP(RIGHT(Z37,4)*1, $A$2:$A$28,$B$2:$B$28)</f>
+        <v>4.973301266935984E-3</v>
       </c>
       <c r="AA40" s="14">
-        <f t="shared" si="6"/>
-        <v>8.8322952876489919E-3</v>
+        <f t="shared" si="12"/>
+        <v>5.7773557920103493E-3</v>
       </c>
       <c r="AB40" s="14">
-        <f t="shared" si="6"/>
-        <v>9.4017469279309204E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28">
+        <f t="shared" si="12"/>
+        <v>6.1614103170847135E-3</v>
+      </c>
+      <c r="AC40" s="14">
+        <f>LOOKUP(RIGHT(AC37,4)*1, $A$2:$A$28,$B$2:$B$28)</f>
+        <v>5.9154648421590773E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1803,55 +2034,55 @@
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41:S41" si="7">LOOKUP(RIGHT(G$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
+        <f t="shared" ref="G41:S41" si="13">LOOKUP(RIGHT(G$37,4)*1, $A$2:$A$16,$B$2:$B$16)</f>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="H41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.8765957446808512E-2</v>
       </c>
       <c r="I41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="J41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.9872340425531916E-2</v>
       </c>
       <c r="L41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.8655319148936171E-2</v>
       </c>
       <c r="M41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.6774468085106383E-2</v>
       </c>
       <c r="N41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.6221276595744681E-2</v>
       </c>
       <c r="O41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="R41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.5100000000000001E-2</v>
       </c>
       <c r="S41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.4299999999999999E-2</v>
       </c>
       <c r="T41">
@@ -1859,54 +2090,58 @@
         <v>2.46E-2</v>
       </c>
       <c r="U41">
-        <f t="shared" ref="U41:AB41" si="8">U40</f>
+        <f t="shared" ref="U41:AB41" si="14">U40</f>
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="V41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2.58E-2</v>
       </c>
       <c r="W41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="X41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="Z41" s="14">
-        <f t="shared" si="8"/>
-        <v>7.8428436473670631E-3</v>
+        <f t="shared" si="14"/>
+        <v>4.973301266935984E-3</v>
       </c>
       <c r="AA41" s="14">
-        <f t="shared" si="8"/>
-        <v>8.8322952876489919E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.7773557920103493E-3</v>
       </c>
       <c r="AB41" s="14">
-        <f t="shared" si="8"/>
-        <v>9.4017469279309204E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28">
+        <f t="shared" si="14"/>
+        <v>6.1614103170847135E-3</v>
+      </c>
+      <c r="AC41" s="14">
+        <f t="shared" ref="AC41" si="15">AC40</f>
+        <v>5.9154648421590773E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:29">
       <c r="B44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:29">
       <c r="A46" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:29">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -1929,7 +2164,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:29">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -1963,4 +2198,269 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CABCAD-E809-2842-A5FF-875B7FF1422B}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>193.4</v>
+      </c>
+      <c r="C3" s="8">
+        <f>H3</f>
+        <v>0.36</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="I3">
+        <f>B3</f>
+        <v>193.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <v>81.7</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="I4">
+        <f>B5</f>
+        <v>232.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>232.1</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="I5">
+        <f>B8</f>
+        <v>158.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>58.1</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="I6">
+        <f>B11</f>
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="8">
+        <f>1-SUM(H3:H6)</f>
+        <v>0.12</v>
+      </c>
+      <c r="I7">
+        <f>B22-SUM(I3:I6)</f>
+        <v>442.20000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>158.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="16">
+        <f>SUMPRODUCT($H$3:$H$7,$I$3:$I$7)/$B$22</f>
+        <v>0.20469474680548982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>13.9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="34">
+      <c r="A18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22">
+        <v>1056.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>